<commit_message>
Minggu 5 Update OOA
</commit_message>
<xml_diff>
--- a/Rabu/Statistika/Minggu 5 - Ukuran Dispersi/Ukuran penyebaran data dari data kelompok.xlsx
+++ b/Rabu/Statistika/Minggu 5 - Ukuran Dispersi/Ukuran penyebaran data dari data kelompok.xlsx
@@ -291,6 +291,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -309,15 +317,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -344,8 +344,8 @@
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="914400" cy="264560"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4"/>
@@ -381,6 +381,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -413,7 +414,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="TextBox 4"/>
@@ -476,8 +477,8 @@
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="914400" cy="367921"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -513,6 +514,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -557,7 +559,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1"/>
@@ -927,28 +929,28 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="15" t="s">
+      <c r="C3" s="14"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="16" t="s">
+      <c r="C4" s="17"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="10" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1002,7 +1004,7 @@
         <v>10</v>
       </c>
       <c r="F7" s="3">
-        <f t="shared" ref="F6:F10" si="0">(B7+D7)/2</f>
+        <f t="shared" ref="F7:F10" si="0">(B7+D7)/2</f>
         <v>63</v>
       </c>
       <c r="H7" s="1" t="s">
@@ -1098,7 +1100,7 @@
   <dimension ref="A2:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:D11"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1107,7 +1109,7 @@
     <col min="2" max="2" width="4.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="3.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="4.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="13.42578125" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="1"/>
     <col min="8" max="8" width="13" style="1" customWidth="1"/>
@@ -1120,40 +1122,40 @@
       </c>
     </row>
     <row r="4" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="18" t="s">
+      <c r="C4" s="14"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
     </row>
     <row r="5" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="19" t="s">
+      <c r="C5" s="17"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="I5" s="12" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1239,7 +1241,7 @@
         <v>630</v>
       </c>
       <c r="H8" s="3">
-        <f t="shared" ref="H7:H11" si="2">ABS(F8-$F$14)</f>
+        <f t="shared" ref="H8:H11" si="2">ABS(F8-$F$14)</f>
         <v>3</v>
       </c>
       <c r="I8" s="3">
@@ -1338,11 +1340,11 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
       <c r="E12" s="3">
         <f>SUM(E6:E11)</f>
         <v>36</v>
@@ -1415,48 +1417,48 @@
       </c>
     </row>
     <row r="4" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="18" t="s">
+      <c r="C4" s="14"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
     </row>
     <row r="5" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="19" t="s">
+      <c r="C5" s="17"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="19" t="s">
+      <c r="F5" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="I5" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="J5" s="19" t="s">
+      <c r="J5" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="K5" s="19" t="s">
+      <c r="K5" s="12" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1558,7 +1560,7 @@
         <v>630</v>
       </c>
       <c r="H8" s="3">
-        <f t="shared" ref="H8:H12" si="4">ABS(F8-$F$14)</f>
+        <f t="shared" ref="H8:H11" si="4">ABS(F8-$F$14)</f>
         <v>3</v>
       </c>
       <c r="I8" s="3">
@@ -1689,11 +1691,11 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
       <c r="E12" s="3">
         <f>SUM(E6:E11)</f>
         <v>36</v>
@@ -1750,22 +1752,22 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="18" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="19" t="s">
+      <c r="C3" s="17"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="12" t="s">
         <v>11</v>
       </c>
       <c r="F3" t="s">

</xml_diff>